<commit_message>
Support of Dione for Ubuntu
</commit_message>
<xml_diff>
--- a/MIPI_deployment.xlsx
+++ b/MIPI_deployment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\germaine\work\rpi\rpi-os\linux_rpi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\germaine\work\rpi\rpi-os\mipi_linux_rpi_eg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6448D55-B82C-4F2A-92BD-F55D919CDE87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E915C172-087B-4916-808D-C2E576812885}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="360" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{D61E0E21-A3C2-41B9-A323-5A81E21B33EC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D61E0E21-A3C2-41B9-A323-5A81E21B33EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Raspberry Pi" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
   <si>
     <t>OK*</t>
   </si>
@@ -325,7 +325,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -358,13 +358,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -831,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58883F95-F127-44D2-A3C1-97E2A72EF605}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,33 +839,36 @@
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
     <col min="3" max="3" width="26.140625" customWidth="1"/>
     <col min="7" max="7" width="27.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="13" t="s">
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="20" t="s">
         <v>3</v>
       </c>
+      <c r="H1" s="22"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="13"/>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="19"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="25"/>
     </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -890,8 +890,11 @@
       <c r="G3" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -913,8 +916,11 @@
       <c r="G4" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="H4" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -936,8 +942,11 @@
       <c r="G5" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="H5" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -959,8 +968,11 @@
       <c r="G6" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="H6" s="3" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -982,8 +994,11 @@
       <c r="G7" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="H7" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1005,8 +1020,11 @@
       <c r="G8" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="H8" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1028,36 +1046,39 @@
       <c r="G9" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="H9" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="15"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="14"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="18"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A10:G10"/>
     <mergeCell ref="A11:G11"/>
-    <mergeCell ref="G1:G2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:F2"/>
+    <mergeCell ref="G1:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1068,7 +1089,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DCCCDB1-1EA5-4151-AA8C-0720347F41D2}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1144,6 +1165,24 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="ddfcbff1-988c-4780-af66-42272a7444f2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5eab2033-26a9-4886-8f5a-efa3f46bf7e3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="ddfcbff1-988c-4780-af66-42272a7444f2">
+      <UserInfo>
+        <DisplayName>Cyril Germaine</DisplayName>
+        <AccountId>370</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100994F61C2E354C24B867AAD14EB9B712B" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="173ead120da22e4d04d58d9334952390">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="5eab2033-26a9-4886-8f5a-efa3f46bf7e3" xmlns:ns3="ddfcbff1-988c-4780-af66-42272a7444f2" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7ed80a0b9a34c83decd038c2f8c861fc" ns2:_="" ns3:_="">
     <xsd:import namespace="5eab2033-26a9-4886-8f5a-efa3f46bf7e3"/>
@@ -1398,24 +1437,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="ddfcbff1-988c-4780-af66-42272a7444f2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5eab2033-26a9-4886-8f5a-efa3f46bf7e3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="ddfcbff1-988c-4780-af66-42272a7444f2">
-      <UserInfo>
-        <DisplayName>Cyril Germaine</DisplayName>
-        <AccountId>370</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21273CB7-CC8A-48C1-BA2A-0CD67C70C578}">
   <ds:schemaRefs>
@@ -1425,6 +1446,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6CC26F4-9ACA-496B-B719-4372C9693134}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="5eab2033-26a9-4886-8f5a-efa3f46bf7e3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="ddfcbff1-988c-4780-af66-42272a7444f2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31B71CDC-0E86-4889-96FE-F63C9CD1A6C7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1441,21 +1479,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6CC26F4-9ACA-496B-B719-4372C9693134}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="5eab2033-26a9-4886-8f5a-efa3f46bf7e3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="ddfcbff1-988c-4780-af66-42272a7444f2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added latest Linux version support
</commit_message>
<xml_diff>
--- a/MIPI_deployment.xlsx
+++ b/MIPI_deployment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyril.germaine\Documents\work\projets\mipi_linux_rpi_eg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE23877A-E03F-4AF0-9616-2353439988E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0326770-AA44-4B43-929A-F7E218B6D4D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D61E0E21-A3C2-41B9-A323-5A81E21B33EC}"/>
   </bookViews>
@@ -134,27 +134,29 @@
 15 pin</t>
   </si>
   <si>
+    <t>22-15 same side (A)</t>
+  </si>
+  <si>
+    <t>15-15 opposite side (B)</t>
+  </si>
+  <si>
+    <t>22-22 opposite side (C)</t>
+  </si>
+  <si>
+    <t>38237 Auvidea | Mouser France</t>
+  </si>
+  <si>
+    <t>Not supported</t>
+  </si>
+  <si>
     <t>2023-12-05 6.1.0-rpi7-rpi-v8
 2024-03-15 6.6.20+rpt-rpi-v8
-2024-07-04 6.6.31+rpt-rpi-v8</t>
-  </si>
-  <si>
-    <t>2024-07-04 6.6.31+rpt-rpi-2712</t>
-  </si>
-  <si>
-    <t>22-15 same side (A)</t>
-  </si>
-  <si>
-    <t>15-15 opposite side (B)</t>
-  </si>
-  <si>
-    <t>22-22 opposite side (C)</t>
-  </si>
-  <si>
-    <t>38237 Auvidea | Mouser France</t>
-  </si>
-  <si>
-    <t>Not supported</t>
+2024-07-04 6.6.31+rpt-rpi-v8
+2025-13-05 6.12.25+rpt-rpi-v8</t>
+  </si>
+  <si>
+    <t>2024-07-04 6.6.31+rpt-rpi-2712
+2025-13-05 6.12.25+rpt-rpi-2712</t>
   </si>
 </sst>
 </file>
@@ -164,7 +166,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -831,18 +833,18 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.375" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.875" customWidth="1"/>
-    <col min="3" max="3" width="26.125" customWidth="1"/>
-    <col min="7" max="7" width="27.375" customWidth="1"/>
-    <col min="8" max="8" width="13.375" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1">
+    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>2</v>
       </c>
@@ -858,7 +860,7 @@
       </c>
       <c r="H1" s="22"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="19"/>
       <c r="B2" s="23"/>
       <c r="C2" s="24"/>
@@ -868,7 +870,7 @@
       <c r="G2" s="23"/>
       <c r="H2" s="25"/>
     </row>
-    <row r="3" spans="1:8" ht="30">
+    <row r="3" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -894,7 +896,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="42.75">
+    <row r="4" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -902,7 +904,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>20</v>
@@ -914,13 +916,13 @@
         <v>19</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -946,7 +948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -972,7 +974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="18" customHeight="1">
+    <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -995,10 +997,10 @@
         <v>0</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="19.5" customHeight="1">
+    <row r="8" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -1021,10 +1023,10 @@
         <v>0</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="18" customHeight="1">
+    <row r="9" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -1047,10 +1049,10 @@
         <v>0</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>12</v>
       </c>
@@ -1061,7 +1063,7 @@
       <c r="F10" s="13"/>
       <c r="G10" s="14"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>22</v>
       </c>
@@ -1093,15 +1095,15 @@
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.75" style="10" customWidth="1"/>
-    <col min="3" max="3" width="21.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="57">
+    <row r="1" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="8" t="s">
         <v>25</v>
@@ -1113,7 +1115,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>23</v>
       </c>
@@ -1121,13 +1123,13 @@
         <v>26</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>24</v>
       </c>
@@ -1135,15 +1137,15 @@
         <v>27</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="24" spans="4:4">
+    <row r="24" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D24" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1156,12 +1158,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="ddfcbff1-988c-4780-af66-42272a7444f2" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5eab2033-26a9-4886-8f5a-efa3f46bf7e3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="ddfcbff1-988c-4780-af66-42272a7444f2">
+      <UserInfo>
+        <DisplayName>Cyril Germaine</DisplayName>
+        <AccountId>370</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1420,27 +1431,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="ddfcbff1-988c-4780-af66-42272a7444f2" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5eab2033-26a9-4886-8f5a-efa3f46bf7e3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="ddfcbff1-988c-4780-af66-42272a7444f2">
-      <UserInfo>
-        <DisplayName>Cyril Germaine</DisplayName>
-        <AccountId>370</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21273CB7-CC8A-48C1-BA2A-0CD67C70C578}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6CC26F4-9ACA-496B-B719-4372C9693134}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="5eab2033-26a9-4886-8f5a-efa3f46bf7e3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="ddfcbff1-988c-4780-af66-42272a7444f2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1465,18 +1476,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C6CC26F4-9ACA-496B-B719-4372C9693134}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21273CB7-CC8A-48C1-BA2A-0CD67C70C578}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="5eab2033-26a9-4886-8f5a-efa3f46bf7e3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="ddfcbff1-988c-4780-af66-42272a7444f2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>